<commit_message>
changed 500 ohm to 510 ohm
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill of Materials.v1.xlsx
+++ b/Bill of Materials/Bill of Materials.v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
   <si>
     <t>Value</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Resistor - 10k ohm</t>
   </si>
   <si>
-    <t>Resistor - 500 ohm</t>
-  </si>
-  <si>
     <t>Resistor - 100 ohm</t>
   </si>
   <si>
@@ -213,16 +210,16 @@
     <t>RC0603JR-0710KL</t>
   </si>
   <si>
-    <t>PLT0603Z5000AST5</t>
-  </si>
-  <si>
-    <t>Vishay Thin Film</t>
-  </si>
-  <si>
     <t>RC0603FR-07100RL</t>
   </si>
   <si>
     <t>RC0603JR-07220RL</t>
+  </si>
+  <si>
+    <t>Resistor - 510 ohm</t>
+  </si>
+  <si>
+    <t>RC0603JR-07510RL</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1032,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,10 +1316,10 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" t="s">
         <v>61</v>
-      </c>
-      <c r="H8" t="s">
-        <v>62</v>
       </c>
       <c r="I8" t="s">
         <v>35</v>
@@ -1357,10 +1354,10 @@
         <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
         <v>35</v>
@@ -1377,7 +1374,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1386,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="1">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -1395,27 +1392,27 @@
         <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
         <v>35</v>
       </c>
       <c r="J10">
-        <v>4.5579999999999998</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="K10">
         <v>25</v>
       </c>
       <c r="L10">
-        <v>113.95</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -1433,10 +1430,10 @@
         <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
         <v>35</v>
@@ -1453,7 +1450,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1471,10 +1468,10 @@
         <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
         <v>35</v>
@@ -1491,7 +1488,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Components for board ordered. Quantity and price and status reflected on the Bill of Materials
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill of Materials.v1.xlsx
+++ b/Bill of Materials/Bill of Materials.v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KKY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home01\shadman\Desktop\School Work\ECE 411\groupxx.github.io\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="81">
   <si>
     <t>Value</t>
   </si>
@@ -51,12 +51,6 @@
     <t xml:space="preserve"> American symbol</t>
   </si>
   <si>
-    <t>CC1005</t>
-  </si>
-  <si>
-    <t>C1005</t>
-  </si>
-  <si>
     <t xml:space="preserve"> European symbol</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>LTST-C171GKT</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>REG1117</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>10nF</t>
-  </si>
-  <si>
     <t>Capacitor - 100nF(0.1uF)</t>
   </si>
   <si>
@@ -177,12 +165,6 @@
     <t>Murarta Eelectronics North America</t>
   </si>
   <si>
-    <t>MCH153FN104ZK</t>
-  </si>
-  <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
     <t>Lite-On Inc.</t>
   </si>
   <si>
@@ -220,13 +202,73 @@
   </si>
   <si>
     <t>RC0603JR-07510RL</t>
+  </si>
+  <si>
+    <t>CL21F104ZBCNNNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics America, Inc.</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>LED Green</t>
+  </si>
+  <si>
+    <t>LED Orange</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>LTST-C170KFKT</t>
+  </si>
+  <si>
+    <t>DIP</t>
+  </si>
+  <si>
+    <t>Wire Pre-Crimped</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Shadman</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Polulu</t>
+  </si>
+  <si>
+    <t>Solid Wire Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,8 +403,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,8 +611,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -658,8 +739,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -702,14 +798,28 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="7" xfId="13" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -743,6 +853,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1029,10 +1140,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,51 +1157,57 @@
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" customWidth="1"/>
     <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1097,7 +1216,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1106,448 +1225,684 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2">
-        <v>0.24299999999999999</v>
+        <v>32</v>
+      </c>
+      <c r="J2" s="4">
+        <v>4.99E-2</v>
       </c>
       <c r="K2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="L2">
-        <v>2.4300000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <f>J2*K2</f>
+        <v>4.99</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K3">
+        <v>30</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L18" si="0">J3*K3</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3">
-        <v>3.9899999999999998E-2</v>
-      </c>
-      <c r="K3">
-        <v>100</v>
-      </c>
-      <c r="L3">
-        <v>3.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
       <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4">
+        <v>32</v>
+      </c>
+      <c r="J4" s="4">
         <v>0.4</v>
       </c>
       <c r="K4">
         <v>10</v>
       </c>
       <c r="L4">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
+      <c r="M4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5">
+        <v>32</v>
+      </c>
+      <c r="J5" s="4">
         <v>0.2</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
+        <v>69</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6">
-        <v>0.39200000000000002</v>
+        <v>32</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.21299999999999999</v>
       </c>
       <c r="K6">
         <v>10</v>
       </c>
       <c r="L6">
-        <v>3.92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2.13</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7">
+        <v>32</v>
+      </c>
+      <c r="J7" s="4">
         <v>0.39200000000000002</v>
       </c>
       <c r="K7">
         <v>10</v>
       </c>
       <c r="L7">
+        <f t="shared" si="0"/>
         <v>3.92</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8">
-        <v>1.4E-2</v>
+        <v>32</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.39200000000000002</v>
       </c>
       <c r="K8">
         <v>10</v>
       </c>
       <c r="L8">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.92</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K9">
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
         <v>56</v>
       </c>
-      <c r="B9" t="s">
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K10">
+        <v>40</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>510</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K12">
+        <v>40</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>220</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K13">
+        <v>40</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K9">
+      <c r="I14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="K14">
         <v>10</v>
       </c>
-      <c r="L9">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1">
-        <v>510</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K10">
-        <v>25</v>
-      </c>
-      <c r="L10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1">
-        <v>100</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K11">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>2.56</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17">
+        <v>50</v>
+      </c>
+      <c r="L17">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>22</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21">
+        <v>4.45</v>
+      </c>
+      <c r="N21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>79</v>
+      </c>
+      <c r="L28">
+        <f>SUM(L2:L27)</f>
+        <v>82.84</v>
+      </c>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>32</v>
+      </c>
+      <c r="K42">
         <v>10</v>
       </c>
-      <c r="L11">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1">
-        <v>220</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K12">
-        <v>25</v>
-      </c>
-      <c r="L12">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I41" t="s">
-        <v>35</v>
-      </c>
-      <c r="K41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G42" t="s">
-        <v>41</v>
-      </c>
-      <c r="I42" t="s">
-        <v>40</v>
-      </c>
-      <c r="K42">
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43">
         <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I43" t="s">
-        <v>35</v>
-      </c>
-      <c r="K43">
-        <v>10</v>
       </c>
     </row>
     <row r="44" spans="7:11" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K44">
         <v>10</v>
       </c>
     </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K45">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" display="http://www.digikey.com/product-detail/en/GRM216R71H103KA01D/490-1664-1-ND/587472"/>
+    <hyperlink ref="H3" r:id="rId2" display="http://digikey.com/Suppliers/us/samsung-electro-mechanics.page?lang=en"/>
+    <hyperlink ref="G6" r:id="rId3" display="http://optoelectronics.liteon.com/upload/download/DS-22-99-0185/S_110_LTST-C170KFKT.pdf"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to the bill of materials. Updated the status of shipment
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill of Materials.v1.xlsx
+++ b/Bill of Materials/Bill of Materials.v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
   <si>
     <t>Value</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Wire Pre-Crimped</t>
   </si>
   <si>
-    <t>Ordered</t>
-  </si>
-  <si>
     <t>Shadman</t>
   </si>
   <si>
@@ -261,7 +258,13 @@
     <t xml:space="preserve">Total </t>
   </si>
   <si>
-    <t>-</t>
+    <t>Shipped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSH Park Board </t>
+  </si>
+  <si>
+    <t>PENDING</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,7 +622,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,7 +809,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -814,10 +823,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1145,7 +1155,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,11 +1253,11 @@
         <f>J2*K2</f>
         <v>4.99</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" t="s">
         <v>73</v>
-      </c>
-      <c r="N2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1285,14 +1295,14 @@
         <v>30</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L18" si="0">J3*K3</f>
+        <f t="shared" ref="L3:L16" si="0">J3*K3</f>
         <v>0.65999999999999992</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" t="s">
         <v>73</v>
-      </c>
-      <c r="N3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1330,11 +1340,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" t="s">
         <v>73</v>
-      </c>
-      <c r="N4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1363,11 +1373,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N5" t="s">
         <v>73</v>
-      </c>
-      <c r="N5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1399,11 +1409,11 @@
         <f t="shared" si="0"/>
         <v>2.13</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" t="s">
         <v>73</v>
-      </c>
-      <c r="N6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1441,11 +1451,11 @@
         <f t="shared" si="0"/>
         <v>3.92</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" t="s">
         <v>73</v>
-      </c>
-      <c r="N7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1483,11 +1493,11 @@
         <f t="shared" si="0"/>
         <v>3.92</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" t="s">
         <v>73</v>
-      </c>
-      <c r="N8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1528,11 +1538,11 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" t="s">
         <v>73</v>
-      </c>
-      <c r="N9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1573,11 +1583,11 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" t="s">
         <v>73</v>
-      </c>
-      <c r="N10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1618,11 +1628,11 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" t="s">
         <v>73</v>
-      </c>
-      <c r="N11" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1663,11 +1673,11 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" t="s">
         <v>73</v>
-      </c>
-      <c r="N12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1708,11 +1718,11 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N13" t="s">
         <v>73</v>
-      </c>
-      <c r="N13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1747,11 +1757,11 @@
         <f t="shared" si="0"/>
         <v>2.56</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14" t="s">
         <v>73</v>
-      </c>
-      <c r="N14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1759,15 +1769,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" t="s">
         <v>73</v>
       </c>
-      <c r="N15" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="A16" t="s">
         <v>38</v>
       </c>
       <c r="I16" t="s">
@@ -1783,15 +1793,15 @@
         <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="M16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" t="s">
         <v>73</v>
       </c>
-      <c r="N16" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="A17" t="s">
         <v>72</v>
       </c>
       <c r="K17">
@@ -1800,16 +1810,16 @@
       <c r="L17">
         <v>9.9499999999999993</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N17" t="s">
         <v>73</v>
       </c>
-      <c r="N17" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>78</v>
+      <c r="A18" t="s">
+        <v>77</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1817,48 +1827,72 @@
       <c r="L18">
         <v>22</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N18" t="s">
         <v>73</v>
       </c>
-      <c r="N18" t="s">
-        <v>74</v>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M19" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>75</v>
       </c>
-      <c r="D20" t="s">
-        <v>76</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>80</v>
+      <c r="L20" s="7">
+        <v>11.38</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="N20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L21">
         <v>4.45</v>
       </c>
+      <c r="M21" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="N21" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="N24" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L28">
         <f>SUM(L2:L27)</f>
-        <v>82.84</v>
+        <v>94.22</v>
       </c>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the BOM with current shipment status and board order
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill of Materials.v1.xlsx
+++ b/Bill of Materials/Bill of Materials.v1.xlsx
@@ -264,7 +264,7 @@
     <t xml:space="preserve">OSH Park Board </t>
   </si>
   <si>
-    <t>PENDING</t>
+    <t>Ordered</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1152,10 +1152,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,6 +1879,12 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>36.799999999999997</v>
+      </c>
       <c r="M24" s="9" t="s">
         <v>81</v>
       </c>
@@ -1892,7 +1898,7 @@
       </c>
       <c r="L28">
         <f>SUM(L2:L27)</f>
-        <v>94.22</v>
+        <v>131.01999999999998</v>
       </c>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made changes to the BOM based on current shipment status
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill of Materials.v1.xlsx
+++ b/Bill of Materials/Bill of Materials.v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
   <si>
     <t>Value</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>Through Hole</t>
-  </si>
-  <si>
     <t>ATMEGA328P</t>
   </si>
   <si>
@@ -264,7 +261,25 @@
     <t xml:space="preserve">OSH Park Board </t>
   </si>
   <si>
-    <t>Ordered</t>
+    <t>Board OSH Park</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Microprocessor</t>
+  </si>
+  <si>
+    <t>Jumper Cables</t>
+  </si>
+  <si>
+    <t>4 Pin Female - Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cables </t>
+  </si>
+  <si>
+    <t>Cables</t>
   </si>
 </sst>
 </file>
@@ -628,7 +643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,12 +1165,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+      <selection pane="topRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,15 +1224,15 @@
         <v>36</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1226,7 +1241,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1235,10 +1250,10 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>32</v>
@@ -1253,16 +1268,16 @@
         <f>J2*K2</f>
         <v>4.99</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>79</v>
+      <c r="M2" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1271,7 +1286,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1280,10 +1295,10 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="I3" t="s">
         <v>32</v>
@@ -1298,11 +1313,11 @@
         <f t="shared" ref="L3:L16" si="0">J3*K3</f>
         <v>0.65999999999999992</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>79</v>
+      <c r="M3" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1325,7 +1340,7 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>
@@ -1340,25 +1355,25 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>79</v>
+      <c r="M4" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
         <v>32</v>
@@ -1373,28 +1388,28 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>79</v>
+      <c r="M5" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
@@ -1409,11 +1424,11 @@
         <f t="shared" si="0"/>
         <v>2.13</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>79</v>
+      <c r="M6" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1433,10 +1448,10 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
         <v>32</v>
@@ -1451,11 +1466,11 @@
         <f t="shared" si="0"/>
         <v>3.92</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>79</v>
+      <c r="M7" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1475,10 +1490,10 @@
         <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
@@ -1493,16 +1508,16 @@
         <f t="shared" si="0"/>
         <v>3.92</v>
       </c>
-      <c r="M8" s="8" t="s">
-        <v>79</v>
+      <c r="M8" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -1520,10 +1535,10 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
         <v>54</v>
-      </c>
-      <c r="H9" t="s">
-        <v>55</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1538,16 +1553,16 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>79</v>
+      <c r="M9" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -1565,10 +1580,10 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" t="s">
         <v>32</v>
@@ -1583,16 +1598,16 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="M10" s="8" t="s">
-        <v>79</v>
+      <c r="M10" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -1610,10 +1625,10 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
         <v>32</v>
@@ -1628,16 +1643,16 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>79</v>
+      <c r="M11" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -1655,10 +1670,10 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
         <v>32</v>
@@ -1673,16 +1688,16 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="M12" s="8" t="s">
-        <v>79</v>
+      <c r="M12" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -1700,10 +1715,10 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
         <v>32</v>
@@ -1718,16 +1733,16 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="M13" s="8" t="s">
-        <v>79</v>
+      <c r="M13" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -1757,11 +1772,11 @@
         <f t="shared" si="0"/>
         <v>2.56</v>
       </c>
-      <c r="M14" s="8" t="s">
-        <v>79</v>
+      <c r="M14" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1770,18 +1785,24 @@
         <v>0</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J16" s="4">
         <v>3.7</v>
@@ -1793,16 +1814,22 @@
         <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
-      <c r="M16" s="8" t="s">
-        <v>79</v>
+      <c r="M16" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" t="s">
+        <v>84</v>
       </c>
       <c r="K17">
         <v>50</v>
@@ -1811,15 +1838,21 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>86</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1827,113 +1860,81 @@
       <c r="L18">
         <v>22</v>
       </c>
-      <c r="M18" s="8" t="s">
-        <v>79</v>
+      <c r="M18" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M19" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
         <v>74</v>
-      </c>
-      <c r="D20" t="s">
-        <v>75</v>
       </c>
       <c r="L20" s="7">
         <v>11.38</v>
       </c>
-      <c r="M20" s="8" t="s">
-        <v>79</v>
+      <c r="M20" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L21">
         <v>4.45</v>
       </c>
-      <c r="M21" s="8" t="s">
-        <v>79</v>
+      <c r="M21" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="N21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K24">
         <v>3</v>
       </c>
       <c r="L24">
         <v>36.799999999999997</v>
       </c>
-      <c r="M24" s="9" t="s">
-        <v>81</v>
+      <c r="M24" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="N24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L28">
         <f>SUM(L2:L27)</f>
         <v>131.01999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G43" t="s">
-        <v>38</v>
-      </c>
-      <c r="I43" t="s">
-        <v>37</v>
-      </c>
-      <c r="K43">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I44" t="s">
-        <v>32</v>
-      </c>
-      <c r="K44">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I45" t="s">
-        <v>32</v>
-      </c>
-      <c r="K45">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>